<commit_message>
Uptaded app to recomend stocks not in portfolio
</commit_message>
<xml_diff>
--- a/target_prices.xlsx
+++ b/target_prices.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b7d072364968bd84/Programming/finances-investing/investments-app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b7d072364968bd84/Programming/finances-investing/app-testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="261" documentId="8_{2759A7E6-2EB7-4028-9137-4DC1A8C5F34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03A984C3-822E-4D9B-959B-0EEA890E89AE}"/>
+  <xr:revisionPtr revIDLastSave="254" documentId="8_{2759A7E6-2EB7-4028-9137-4DC1A8C5F34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C2F3F78-1FB4-44EE-99FE-0390A5178495}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AFBED600-4DD2-45FB-B9DB-9C48D54FF126}"/>
   </bookViews>
@@ -723,8 +723,8 @@
   <dimension ref="B2:I74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.5703125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>